<commit_message>
pm2_ecorecover final result for manuscript
</commit_message>
<xml_diff>
--- a/exposan/pm2_ecorecover/data/initial_conditition_calc._cali.xlsx
+++ b/exposan/pm2_ecorecover/data/initial_conditition_calc._cali.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Downloads\EXPOsan\exposan\pm2_ecorecover\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FF93C3B-FAA3-4CB0-8F6F-71630CB0350B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{748695A2-1691-40B7-93FB-C7D64574AB34}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12180" activeTab="2" xr2:uid="{DDF619FE-EB2A-46FB-BA68-BAD48C3E9660}"/>
   </bookViews>
@@ -417,7 +417,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="58">
   <si>
     <t>at Day0 (2022-03-12  12:00:00 AM)</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -615,6 +615,26 @@
   <si>
     <t>at Day5</t>
     <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Q_INF</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>(used for SCADA yield calc.)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PBR</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MEV</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>RET</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -843,22 +863,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:colOff>448236</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>78441</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>542468</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>75462</xdr:rowOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>58130</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>201536</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="그림 2">
+        <xdr:cNvPr id="2" name="그림 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{668B8825-6C15-4DF3-9B59-4685D497AF26}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89C59455-CA90-4FD9-A964-058EB992BC34}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -874,8 +894,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14192250" y="5695950"/>
-          <a:ext cx="3657143" cy="5904762"/>
+          <a:off x="14287501" y="504265"/>
+          <a:ext cx="3711247" cy="6084624"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -886,23 +906,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>672353</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>89646</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>32</xdr:col>
-      <xdr:colOff>4929</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>132679</xdr:rowOff>
+      <xdr:colOff>39984</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>116194</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="그림 3">
+        <xdr:cNvPr id="8" name="그림 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2685BCEC-9D39-4305-BDDB-1B5B4D3F5128}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5502FEBA-7814-4D64-B630-6B9F4D4F8FD6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -918,8 +938,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17992725" y="5657850"/>
-          <a:ext cx="4114286" cy="5371429"/>
+          <a:off x="17929412" y="515470"/>
+          <a:ext cx="4152543" cy="5562253"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -930,23 +950,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>32</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>672353</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>78441</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>38</xdr:col>
-      <xdr:colOff>485200</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>123155</xdr:rowOff>
+      <xdr:colOff>544746</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>152608</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="그림 4">
+        <xdr:cNvPr id="9" name="그림 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7F18F36D-F053-4174-8B84-37AA0FACE599}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C524BB4-442F-4D3F-8023-86E195B4A7FA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -962,8 +982,52 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="22107525" y="5657850"/>
-          <a:ext cx="4600000" cy="5361905"/>
+          <a:off x="22030765" y="504265"/>
+          <a:ext cx="4657305" cy="5609872"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>493058</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>112059</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>44</xdr:col>
+      <xdr:colOff>302952</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>205273</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="그림 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6770A655-2B59-4B29-AB46-1F17244F9F4F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="26636382" y="324971"/>
+          <a:ext cx="3911246" cy="5628920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -974,10 +1038,10 @@
   </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>35379</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>187779</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>334736</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>160564</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1105431" cy="530658"/>
     <xdr:sp macro="" textlink="">
@@ -993,7 +1057,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="16527236" y="8964386"/>
+          <a:off x="16146236" y="2609850"/>
           <a:ext cx="1105431" cy="530658"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1042,9 +1106,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>30</xdr:col>
-      <xdr:colOff>157843</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>187778</xdr:rowOff>
+      <xdr:colOff>375556</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>187777</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1105431" cy="530658"/>
     <xdr:sp macro="" textlink="">
@@ -1060,7 +1124,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="20731843" y="8964385"/>
+          <a:off x="20949556" y="2841170"/>
           <a:ext cx="1105431" cy="530658"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1106,6 +1170,285 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>78920</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>204106</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1105431" cy="530658"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="TextBox 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CAA6849-497F-4649-A956-BDC6409A9EB2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="25415420" y="2857499"/>
+          <a:ext cx="1105431" cy="530658"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="2800" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>X 35.4</a:t>
+          </a:r>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="2800" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FFFF00"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>473214</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>157798</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="그림 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7CE12F09-69DE-41D3-8EF4-DFC0C4E33D3F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="26697214" y="5715000"/>
+          <a:ext cx="2514286" cy="361905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>44824</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>537882</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>51548</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="직선 화살표 연결선 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C34E117-E520-4DB9-A0CF-EFB5318DDCE0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="17106900" y="2599765"/>
+          <a:ext cx="1371600" cy="6724"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FFFF00"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>208430</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>499782</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>2242</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="20" name="직선 화살표 연결선 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4E998BD8-1A97-48E6-8A64-CD7361986E0B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="21170153" y="2550459"/>
+          <a:ext cx="1371600" cy="6724"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FFFF00"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>412377</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>2242</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>416860</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>8966</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="21" name="직선 화살표 연결선 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5E7369A-5F21-4180-A78C-9AC18C55C7B6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="25872142" y="2344271"/>
+          <a:ext cx="1371600" cy="6724"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FFFF00"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2610,10 +2953,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62B58F2C-516A-4DC7-8CC2-83495AB979A0}">
-  <dimension ref="A1:T37"/>
+  <dimension ref="A1:AP37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Y33" sqref="Y33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2622,12 +2965,23 @@
     <col min="2" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="W2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -2635,7 +2989,7 @@
         <v>35.804091778642068</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -2643,7 +2997,7 @@
         <v>0.35744153755741681</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -2657,7 +3011,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -2676,13 +3030,13 @@
         <v>552.21030897427556</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="18"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
@@ -2723,7 +3077,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
@@ -2773,7 +3127,7 @@
         <v>0.1913384581420968</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>21</v>
       </c>
@@ -2823,7 +3177,7 @@
         <v>0.1913384581420968</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
@@ -2873,7 +3227,7 @@
         <v>0.31570845593445968</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
@@ -2923,7 +3277,7 @@
         <v>0.23993842651018937</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
@@ -2938,7 +3292,7 @@
       <c r="M15" s="4"/>
       <c r="N15" s="4"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
         <v>24</v>
       </c>
@@ -2955,21 +3309,21 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:41" x14ac:dyDescent="0.3">
       <c r="B17" s="5">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="D17" s="6"/>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:41" x14ac:dyDescent="0.3">
       <c r="E19" s="6"/>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>27</v>
       </c>
@@ -2983,7 +3337,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <f>B6</f>
         <v>845.53361404097905</v>
@@ -2999,10 +3353,10 @@
         <v>1.7000000000000001E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:41" x14ac:dyDescent="0.3">
       <c r="F25" s="7"/>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:41" x14ac:dyDescent="0.3">
       <c r="B26" s="8"/>
       <c r="C26" s="9">
         <v>0.15</v>
@@ -3027,7 +3381,7 @@
       <c r="Q26" s="8"/>
       <c r="R26" s="8"/>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:41" x14ac:dyDescent="0.3">
       <c r="B27" s="8"/>
       <c r="C27" s="8" t="s">
         <v>31</v>
@@ -3068,7 +3422,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="28" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:41" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B28" s="12"/>
       <c r="C28" s="12"/>
       <c r="D28" s="12"/>
@@ -3087,7 +3441,7 @@
       <c r="Q28" s="12"/>
       <c r="R28" s="12"/>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:41" x14ac:dyDescent="0.3">
       <c r="B29" s="13">
         <v>0</v>
       </c>
@@ -3141,12 +3495,12 @@
         <v>634.48842397635076</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:41" x14ac:dyDescent="0.3">
       <c r="T31" s="17" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:41" x14ac:dyDescent="0.3">
       <c r="C32" s="1" t="s">
         <v>42</v>
       </c>
@@ -3175,8 +3529,14 @@
         <f>SUM(K32,O32,R32,G33,G37)</f>
         <v>537.88652209603288</v>
       </c>
-    </row>
-    <row r="33" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="AN32" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AO32" s="1">
+        <v>449.06</v>
+      </c>
+    </row>
+    <row r="33" spans="3:42" x14ac:dyDescent="0.3">
       <c r="C33" s="1">
         <f>B24*D24</f>
         <v>55.841491918746968</v>
@@ -3194,7 +3554,16 @@
         <v>8.8383261194029825E-2</v>
       </c>
     </row>
-    <row r="36" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:42" x14ac:dyDescent="0.3">
+      <c r="AO34" s="1">
+        <f>0.52616/449.06</f>
+        <v>1.1716919788001602E-3</v>
+      </c>
+      <c r="AP34" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="36" spans="3:42" x14ac:dyDescent="0.3">
       <c r="C36" s="1" t="s">
         <v>45</v>
       </c>
@@ -3208,7 +3577,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="37" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:42" x14ac:dyDescent="0.3">
       <c r="C37" s="1">
         <f>B24*F24</f>
         <v>10.547837362429984</v>

</xml_diff>